<commit_message>
menu page test case written
</commit_message>
<xml_diff>
--- a/test_case_report/sprint_46.xlsx
+++ b/test_case_report/sprint_46.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\office\SymlexVPNTestCases\test_case_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1820DCF0-79DC-4E2A-AD87-06569FB5E377}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2174425A-1F3D-4F9F-BA0A-FEFD498914EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -535,7 +535,7 @@
   <dimension ref="B2:C60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57:C57"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -584,19 +584,25 @@
       <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="2">
+        <v>7280</v>
+      </c>
     </row>
     <row r="10" spans="2:3" ht="18">
       <c r="B10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4">
+        <v>3160</v>
+      </c>
     </row>
     <row r="11" spans="2:3" ht="18">
       <c r="B11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="5">
+        <v>3160</v>
+      </c>
     </row>
     <row r="14" spans="2:3" ht="18.75" customHeight="1">
       <c r="B14" s="6" t="s">
@@ -608,19 +614,25 @@
       <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2">
+        <v>7300</v>
+      </c>
     </row>
     <row r="16" spans="2:3" ht="18">
       <c r="B16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4">
+        <v>3120</v>
+      </c>
     </row>
     <row r="17" spans="2:3" ht="18">
       <c r="B17" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="5">
+        <v>3120</v>
+      </c>
     </row>
     <row r="20" spans="2:3" ht="18">
       <c r="B20" s="6" t="s">
@@ -792,16 +804,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B26:C26"/>
     <mergeCell ref="B32:C32"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B50:C50"/>
     <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B26:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
symlex android purchase page UI test case wriiten
</commit_message>
<xml_diff>
--- a/test_case_report/sprint_46.xlsx
+++ b/test_case_report/sprint_46.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\office\SymlexVPNTestCases\test_case_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E8DFE7-985F-48CE-919E-63D476A8A9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3CC581-F923-4E8F-AFE3-DEA052350976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -538,7 +538,7 @@
   <dimension ref="B2:C60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -789,19 +789,25 @@
       <c r="B51" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C51" s="2"/>
+      <c r="C51" s="2">
+        <v>7322</v>
+      </c>
     </row>
     <row r="52" spans="2:3" ht="18">
       <c r="B52" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C52" s="4"/>
+      <c r="C52" s="4">
+        <v>3220</v>
+      </c>
     </row>
     <row r="53" spans="2:3" ht="18">
       <c r="B53" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="5"/>
+      <c r="C53" s="5">
+        <v>3220</v>
+      </c>
     </row>
     <row r="57" spans="2:3" ht="18">
       <c r="B57" s="6" t="s">
@@ -829,16 +835,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B57:C57"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B57:C57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>